<commit_message>
Github source update for Vol2
</commit_message>
<xml_diff>
--- a/App_Data/XlsIO/ExcelTopdfwithChart.xlsx
+++ b/App_Data/XlsIO/ExcelTopdfwithChart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Syncfusion\Windows\16.3.0.29\Common\Data\XlsIO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Gitlab\EJ2-27843-XlsIOChangesHotFix\App_Data\XlsIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EDB6F0DF-186A-40B8-87C6-A004A90FA48A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F24B26F-1BAA-486F-AE99-C0BC63B1653B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TableStyle" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Excel 2016 Chart" sheetId="9" r:id="rId4"/>
     <sheet name="Autoshapes" sheetId="10" r:id="rId5"/>
     <sheet name="GroupShapes" sheetId="11" r:id="rId6"/>
-    <sheet name="Picture Recolor" sheetId="12" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="__IntlFixup" hidden="1">TRUE</definedName>
@@ -47,12 +46,19 @@
     <definedName name="Macro2">Macro2</definedName>
     <definedName name="Ownership" hidden="1">OFFSET(Data.Top.Left,1,0)</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="189">
   <si>
     <t>3 Self-Promotion</t>
   </si>
@@ -619,24 +625,6 @@
   </si>
   <si>
     <t>Closed Sales</t>
-  </si>
-  <si>
-    <t>Gray Scale</t>
-  </si>
-  <si>
-    <t>Color Change</t>
-  </si>
-  <si>
-    <t>Original Picture</t>
-  </si>
-  <si>
-    <t>Black And White</t>
-  </si>
-  <si>
-    <t>Duotone</t>
-  </si>
-  <si>
-    <t>Picture Recolor</t>
   </si>
 </sst>
 </file>
@@ -656,7 +644,7 @@
     <numFmt numFmtId="170" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="171" formatCode="#,##0_ "/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="28">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -812,20 +800,8 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <b/>
-      <sz val="36"/>
-      <color rgb="FF0070C0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="17">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -913,12 +889,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF5786B9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1239,7 +1209,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="34" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="34" applyFont="1" applyFill="1"/>
@@ -1342,12 +1312,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5664,520 +5628,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>3907</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>109085</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>604958</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>158435</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Picture 19">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD78E1BB-B739-42EC-BF2D-1FF28856518A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FF0000"/>
-            </a:clrTo>
-          </a:clrChange>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7319107" y="4776335"/>
-          <a:ext cx="1820251" cy="1636850"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6930</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>18453</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>607945</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>150353</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Picture 20">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9A092C8-3942-4099-8D93-D73067BA01DB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="616530" y="6273203"/>
-          <a:ext cx="1820215" cy="1624150"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>10429</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>116599</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>405</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>154699</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Picture 21">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C136BF78-8D97-4DD6-B1AE-176DE5C7C00E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:grayscl/>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7406311" y="9697628"/>
-          <a:ext cx="1838947" cy="1718982"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>13144</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>105051</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>3120</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>149501</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Picture 23">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BAD3D00-4243-45F7-A100-D1E02EDF63C4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:biLevel thresh="50000"/>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7409026" y="2626375"/>
-          <a:ext cx="1838947" cy="1725332"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>7039</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>23826</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>342</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>154288</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="Picture 25">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5325517C-678D-443B-A9A0-2DA9A045A259}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:duotone>
-            <a:schemeClr val="accent1">
-              <a:shade val="45000"/>
-              <a:satMod val="135000"/>
-            </a:schemeClr>
-            <a:prstClr val="white"/>
-          </a:duotone>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7322239" y="7135826"/>
-          <a:ext cx="1822103" cy="1622712"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>15875</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>62914</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>65802</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE52841B-32DF-4FA7-852C-CA330AAB1E65}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm flipV="1">
-          <a:off x="2481169" y="4097032"/>
-          <a:ext cx="4914713" cy="3196564"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
-        </a:solidFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="808080"/>
-                </a:outerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>606137</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>57720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>11546</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>80813</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="29" name="Straight Arrow Connector 28">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E107341B-B9F1-409B-82ED-7508EC071BBE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm flipV="1">
-          <a:off x="2455108" y="6108896"/>
-          <a:ext cx="4952320" cy="1199711"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
-        </a:solidFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="808080"/>
-                </a:outerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>608446</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>83122</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>62916</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="30" name="Straight Arrow Connector 29">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11B7A17F-0E2D-44AA-891D-83C13286C161}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2457417" y="7310916"/>
-          <a:ext cx="4938465" cy="2669206"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
-        </a:solidFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="808080"/>
-                </a:outerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>9580</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>133150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>7039</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>35083</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="31" name="Straight Arrow Connector 30">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D1C7A28-D4D9-4F2F-AAC6-93370F691114}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:endCxn id="26" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2447980" y="7086400"/>
-          <a:ext cx="4874259" cy="854433"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
-        </a:solidFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="808080"/>
-                </a:outerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F99" totalsRowShown="0">
   <autoFilter ref="A1:F99" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
@@ -11928,7 +11378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3B4258-EABF-44CA-93FA-8274679CD328}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
@@ -11938,154 +11388,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F13C84E-E0AC-4332-A65E-80C5971F909C}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:O69"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5"/>
-  <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="40" t="s">
-        <v>194</v>
-      </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="40"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
-    </row>
-    <row r="27" spans="13:15" ht="17.5">
-      <c r="M27" s="41" t="s">
-        <v>192</v>
-      </c>
-      <c r="N27" s="41"/>
-      <c r="O27" s="41"/>
-    </row>
-    <row r="41" spans="13:15" ht="17.5">
-      <c r="M41" s="41" t="s">
-        <v>190</v>
-      </c>
-      <c r="N41" s="41"/>
-      <c r="O41" s="41"/>
-    </row>
-    <row r="50" spans="2:15" ht="17.5">
-      <c r="B50" s="41" t="s">
-        <v>191</v>
-      </c>
-      <c r="C50" s="41"/>
-      <c r="D50" s="41"/>
-    </row>
-    <row r="55" spans="2:15" ht="17.5">
-      <c r="M55" s="41" t="s">
-        <v>193</v>
-      </c>
-      <c r="N55" s="41"/>
-      <c r="O55" s="41"/>
-    </row>
-    <row r="69" spans="13:15" ht="17.5">
-      <c r="M69" s="41" t="s">
-        <v>189</v>
-      </c>
-      <c r="N69" s="41"/>
-      <c r="O69" s="41"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:O5"/>
-    <mergeCell ref="M41:O41"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="M69:O69"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="M55:O55"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="66" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>